<commit_message>
Changes in Dox and Box
</commit_message>
<xml_diff>
--- a/controller/Excel/request.xlsx
+++ b/controller/Excel/request.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,35 +427,18 @@
         <v>ACCOUNT MANUAL</v>
       </c>
       <c r="C2" t="str">
-        <v>dfs</v>
+        <v>jhjh</v>
       </c>
       <c r="D2" t="str">
-        <v>Physical-Returnable</v>
+        <v>Digital (Scan)</v>
       </c>
       <c r="E2" t="str">
-        <v>Urgent</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>F-000001160</v>
-      </c>
-      <c r="B3" t="str">
-        <v>ACCOUNT MANUAL</v>
-      </c>
-      <c r="C3" t="str">
-        <v>dfs</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Physical-Returnable</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Urgent</v>
+        <v>Standard</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>